<commit_message>
Implement custom agggregate sector mapping
- General creation of smaller, more purposed functions
- Map instructions to custom sector map
- Map user data to custom sector map
- Use default extension data to calculate breakdowns in user data
</commit_message>
<xml_diff>
--- a/input/extension/user-defined-energy/E.US-EIA_inventory_aggsec-mapping.xlsx
+++ b/input/extension/user-defined-energy/E.US-EIA_inventory_aggsec-mapping.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26709"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ben/mystuff/CEDS/input/extension/user-defined-energy/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brau074\Documents\CEDS2\CEDS\input\extension\user-defined-energy\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12700" yWindow="460" windowWidth="16100" windowHeight="17440" tabRatio="500"/>
+    <workbookView xWindow="12705" yWindow="465" windowWidth="16095" windowHeight="17445" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="agg_sector" sheetId="2" r:id="rId1"/>
-    <sheet name="agg_fuel" sheetId="4" r:id="rId2"/>
+    <sheet name="agg_fuel" sheetId="4" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -25,31 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
-  <si>
-    <t>sector</t>
-  </si>
-  <si>
-    <t>agg_sector</t>
-  </si>
-  <si>
-    <t>Transportation</t>
-  </si>
-  <si>
-    <t>1A3_Transportation</t>
-  </si>
-  <si>
-    <t>Industry</t>
-  </si>
-  <si>
-    <t>Energy Transf/Ext</t>
-  </si>
-  <si>
-    <t>1A2_Industry-combustion</t>
-  </si>
-  <si>
-    <t>1A1_Energy-transformation</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
   <si>
     <t>fuel</t>
   </si>
@@ -113,6 +88,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -381,102 +359,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>